<commit_message>
WIP snapshot before recovery - 2025-10-17
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\OneDrive\Documentos\Ortopedia Cuernavaca\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\OneDrive\Documentos\Ortopedia Cuernavaca\ortotech-vite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B7B5E82-F894-46CF-9720-4E9D89568B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1363E10-BE43-4B06-A441-4A58843C7D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="28800" windowHeight="15370" xr2:uid="{A6460276-EAF4-470B-BF5A-F452FBD3DC68}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A6460276-EAF4-470B-BF5A-F452FBD3DC68}"/>
   </bookViews>
   <sheets>
     <sheet name="Zona A" sheetId="2" r:id="rId1"/>
@@ -1242,10 +1242,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1587,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3FDF0FA-53B1-4F7F-A8A4-3496CCE9C029}">
   <dimension ref="A1:K259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D259" sqref="D259"/>
+    <sheetView tabSelected="1" topLeftCell="A220" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>